<commit_message>
mise a jour ppt et Excel
</commit_message>
<xml_diff>
--- a/Café.xlsx
+++ b/Café.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noafoucoux/Documents/Cours/ma2/aidmulticrit/projetaidmulticrit/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ingri\Ma1\AMCD\projetaidmulticrit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61878F3A-C5E0-0B45-87A9-2508A63B29FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68EE0E71-74D3-42A5-ABAB-1E3AB9235540}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="1" xr2:uid="{E16892A5-2733-6247-BC2F-556276338AEC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="4" xr2:uid="{E16892A5-2733-6247-BC2F-556276338AEC}"/>
   </bookViews>
   <sheets>
     <sheet name="Dominance" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="42">
   <si>
     <t>BEKO CEG3190B</t>
   </si>
@@ -180,12 +180,21 @@
   <si>
     <t>=&gt; PQ ? Car on veut avoir 0,3 et 0,3 absolument et soit mousse et température ou capacité du reservoir'</t>
   </si>
+  <si>
+    <t>poids</t>
+  </si>
+  <si>
+    <t>Normalisat°</t>
+  </si>
+  <si>
+    <t>Utilité Additive</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -238,6 +247,12 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Damascus Regular"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
     </font>
   </fonts>
   <fills count="8">
@@ -562,7 +577,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -608,7 +623,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
@@ -621,6 +635,11 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -657,7 +676,7 @@
       <font>
         <b val="0"/>
         <i val="0"/>
-        <color rgb="FFFFC000"/>
+        <color theme="5"/>
       </font>
     </dxf>
   </dxfs>
@@ -2074,31 +2093,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>97.251135786818494</c:v>
+                  <c:v>70.899645951661682</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>69.811743989590497</c:v>
+                  <c:v>50.73981964406417</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>75.790749292928581</c:v>
+                  <c:v>55.3488698183574</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>62.807514409823796</c:v>
+                  <c:v>42.365634935252615</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>66.389096446542354</c:v>
+                  <c:v>41.246390548778066</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>63.702909919003439</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>65.71754981465763</c:v>
+                  <c:v>41.246390548778066</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>81.899583363515632</c:v>
+                  <c:v>60.11461062517499</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>30.443447312107772</c:v>
+                  <c:v>4.6291947824587503</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5552,22 +5571,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{078AD970-769F-5440-BD83-72826FE4EE68}">
   <dimension ref="A1:X27"/>
   <sheetViews>
-    <sheetView topLeftCell="F7" zoomScale="86" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+    <sheetView topLeftCell="D1" zoomScale="56" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6"/>
   <cols>
-    <col min="9" max="9" width="39.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="32.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="35" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="29.1640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="39.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="32.5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24" customWidth="1"/>
+    <col min="10" max="10" width="14.796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.19921875" customWidth="1"/>
+    <col min="12" max="12" width="15.09765625" customWidth="1"/>
+    <col min="13" max="15" width="15.19921875" customWidth="1"/>
+    <col min="16" max="18" width="15.09765625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24">
@@ -6579,6 +6594,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6586,20 +6602,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41137E64-42F2-044D-BD17-AF19D2ABB3C0}">
   <dimension ref="A1:O72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D10" zoomScale="69" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Y52" sqref="Y52"/>
+    <sheetView topLeftCell="B1" zoomScale="67" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6"/>
   <cols>
-    <col min="2" max="2" width="43.1640625" customWidth="1"/>
-    <col min="3" max="3" width="17.83203125" customWidth="1"/>
-    <col min="4" max="5" width="13.6640625" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" style="9"/>
-    <col min="13" max="13" width="10.83203125" style="28"/>
+    <col min="2" max="2" width="43.19921875" customWidth="1"/>
+    <col min="3" max="3" width="17.796875" customWidth="1"/>
+    <col min="4" max="5" width="13.69921875" customWidth="1"/>
+    <col min="6" max="6" width="11.296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.8984375" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="11.296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.296875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.8984375" style="28" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="11.296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:15">
       <c r="C1" t="s">
         <v>11</v>
       </c>
@@ -6630,8 +6651,15 @@
       <c r="L1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:14">
+      <c r="M1" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="N1" s="61" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1" s="61"/>
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -6673,16 +6701,15 @@
         <f t="shared" ref="L2:L18" ca="1" si="3">_xlfn.FORECAST.LINEAR(G2,OFFSET(L$26:L$27,MATCH(G2,G$26:G$27,1)-1,0,2),OFFSET(G$26:G$27,MATCH(G2,G$26:G$27,1)-1,0,2))</f>
         <v>100</v>
       </c>
-      <c r="M2" s="28" cm="1">
-        <f t="array" aca="1" ref="M2" ca="1">MMULT(H2:K2,TRANSPOSE(H$19:K$19))</f>
-        <v>97.251135786818494</v>
+      <c r="M2" s="28">
+        <v>70.899645951661682</v>
       </c>
       <c r="N2">
-        <f ca="1">RANK(M2,M$2:M$10)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14">
+        <f>RANK(M2,M$2:M$10)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -6724,16 +6751,15 @@
         <f t="shared" ca="1" si="3"/>
         <v>72.375127420998979</v>
       </c>
-      <c r="M3" s="28" cm="1">
-        <f t="array" aca="1" ref="M3" ca="1">MMULT(H3:K3,TRANSPOSE(H$19:K$19))</f>
-        <v>69.811743989590497</v>
+      <c r="M3" s="28">
+        <v>50.73981964406417</v>
       </c>
       <c r="N3">
-        <f t="shared" ref="N3:N10" ca="1" si="5">RANK(M3,M$2:M$10)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14">
+        <f t="shared" ref="N3:N10" si="5">RANK(M3,M$2:M$10)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -6775,16 +6801,15 @@
         <f t="shared" ca="1" si="3"/>
         <v>77.573904179408771</v>
       </c>
-      <c r="M4" s="28" cm="1">
-        <f t="array" aca="1" ref="M4" ca="1">MMULT(H4:K4,TRANSPOSE(H$19:K$19))</f>
-        <v>75.790749292928581</v>
+      <c r="M4" s="28">
+        <v>55.3488698183574</v>
       </c>
       <c r="N4">
-        <f t="shared" ca="1" si="5"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -6826,16 +6851,15 @@
         <f t="shared" ca="1" si="3"/>
         <v>77.573904179408771</v>
       </c>
-      <c r="M5" s="28" cm="1">
-        <f t="array" aca="1" ref="M5" ca="1">MMULT(H5:K5,TRANSPOSE(H$19:K$19))</f>
-        <v>62.807514409823796</v>
+      <c r="M5" s="28">
+        <v>42.365634935252615</v>
       </c>
       <c r="N5">
-        <f t="shared" ca="1" si="5"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -6877,16 +6901,15 @@
         <f t="shared" ca="1" si="3"/>
         <v>95.412844036697251</v>
       </c>
-      <c r="M6" s="28" cm="1">
-        <f t="array" aca="1" ref="M6" ca="1">MMULT(H6:K6,TRANSPOSE(H$19:K$19))</f>
-        <v>66.389096446542354</v>
+      <c r="M6" s="28">
+        <v>41.246390548778066</v>
       </c>
       <c r="N6">
-        <f t="shared" ca="1" si="5"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -6928,16 +6951,15 @@
         <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
-      <c r="M7" s="28" cm="1">
-        <f t="array" aca="1" ref="M7" ca="1">MMULT(H7:K7,TRANSPOSE(H$19:K$19))</f>
+      <c r="M7" s="28">
         <v>63.702909919003439</v>
       </c>
       <c r="N7">
-        <f t="shared" ca="1" si="5"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -6979,16 +7001,15 @@
         <f t="shared" ca="1" si="3"/>
         <v>92.864424057084619</v>
       </c>
-      <c r="M8" s="28" cm="1">
-        <f t="array" aca="1" ref="M8" ca="1">MMULT(H8:K8,TRANSPOSE(H$19:K$19))</f>
-        <v>65.71754981465763</v>
+      <c r="M8" s="28">
+        <v>41.246390548778066</v>
       </c>
       <c r="N8">
-        <f t="shared" ca="1" si="5"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -7027,19 +7048,18 @@
         <v>44.444444444444429</v>
       </c>
       <c r="L9">
-        <f t="shared" ca="1" si="3"/>
+        <f ca="1">_xlfn.FORECAST.LINEAR(G9,OFFSET(L$26:L$27,MATCH(G9,G$26:G$27,1)-1,0,2),OFFSET(G$26:G$27,MATCH(G9,G$26:G$27,1)-1,0,2))</f>
         <v>82.670744138634049</v>
       </c>
-      <c r="M9" s="28" cm="1">
-        <f t="array" aca="1" ref="M9" ca="1">MMULT(H9:K9,TRANSPOSE(H$19:K$19))</f>
-        <v>81.899583363515632</v>
+      <c r="M9" s="28">
+        <v>60.11461062517499</v>
       </c>
       <c r="N9">
-        <f t="shared" ca="1" si="5"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" ht="17" thickBot="1">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="16.2" thickBot="1">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -7081,16 +7101,15 @@
         <f t="shared" ca="1" si="3"/>
         <v>97.961264016309883</v>
       </c>
-      <c r="M10" s="28" cm="1">
-        <f t="array" aca="1" ref="M10" ca="1">MMULT(H10:K10,TRANSPOSE(H$19:K$19))</f>
-        <v>30.443447312107772</v>
+      <c r="M10" s="28">
+        <v>4.6291947824587503</v>
       </c>
       <c r="N10">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:14" s="14" customFormat="1">
+    <row r="11" spans="1:15" s="14" customFormat="1">
       <c r="A11" s="12"/>
       <c r="B11" s="12"/>
       <c r="C11" s="15"/>
@@ -7115,7 +7134,7 @@
       </c>
       <c r="M11" s="29"/>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:15">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="16"/>
@@ -7139,7 +7158,7 @@
         <v>67.278287461773701</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:15">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="16"/>
@@ -7163,7 +7182,7 @@
         <v>92.762487257900105</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:15">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="16"/>
@@ -7187,7 +7206,7 @@
         <v>82.568807339449535</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:15">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="16"/>
@@ -7211,7 +7230,7 @@
         <v>92.762487257900105</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:15">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="16"/>
@@ -7259,7 +7278,7 @@
         <v>92.762487257900105</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="17" thickBot="1">
+    <row r="18" spans="1:15" ht="16.2" thickBot="1">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1">
@@ -7290,7 +7309,9 @@
       <c r="D19" s="12"/>
       <c r="E19" s="12"/>
       <c r="F19" s="12"/>
-      <c r="G19" s="13"/>
+      <c r="G19" s="60" t="s">
+        <v>40</v>
+      </c>
       <c r="H19" s="14">
         <f ca="1">H20/SUM($H20:$L20)</f>
         <v>0.17907910183592804</v>
@@ -7314,7 +7335,9 @@
       <c r="M19" s="29"/>
     </row>
     <row r="20" spans="1:15">
-      <c r="G20" s="10"/>
+      <c r="G20" s="59" t="s">
+        <v>39</v>
+      </c>
       <c r="H20">
         <f ca="1">(L17-L18)/(H17-H18)</f>
         <v>-0.67957866123003752</v>
@@ -7335,7 +7358,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:15" s="20" customFormat="1" ht="17" thickBot="1">
+    <row r="21" spans="1:15" s="20" customFormat="1" ht="16.2" thickBot="1">
       <c r="G21" s="21"/>
       <c r="M21" s="40"/>
     </row>
@@ -7461,7 +7484,7 @@
         <v>9</v>
       </c>
       <c r="O26">
-        <f t="shared" ref="O26:O35" si="7">(N25-1)*100/$N$26</f>
+        <f>(N25-1)*100/$N$26</f>
         <v>100</v>
       </c>
     </row>
@@ -7500,7 +7523,7 @@
         <v>8</v>
       </c>
       <c r="O27">
-        <f t="shared" si="7"/>
+        <f>(N26-1)*100/$N$26</f>
         <v>88.888888888888886</v>
       </c>
     </row>
@@ -7539,7 +7562,7 @@
         <v>7</v>
       </c>
       <c r="O28">
-        <f t="shared" si="7"/>
+        <f>(N27-1)*100/$N$26</f>
         <v>77.777777777777771</v>
       </c>
     </row>
@@ -7572,7 +7595,7 @@
         <v>6</v>
       </c>
       <c r="O29">
-        <f t="shared" si="7"/>
+        <f>(N28-1)*100/$N$26</f>
         <v>66.666666666666671</v>
       </c>
     </row>
@@ -7605,7 +7628,7 @@
         <v>5</v>
       </c>
       <c r="O30">
-        <f t="shared" si="7"/>
+        <f>(N29-1)*100/$N$26</f>
         <v>55.555555555555557</v>
       </c>
     </row>
@@ -7638,7 +7661,7 @@
         <v>4</v>
       </c>
       <c r="O31">
-        <f t="shared" si="7"/>
+        <f>(N30-1)*100/$N$26</f>
         <v>44.444444444444443</v>
       </c>
     </row>
@@ -7653,7 +7676,7 @@
         <v>3</v>
       </c>
       <c r="O32">
-        <f t="shared" si="7"/>
+        <f>(N31-1)*100/$N$26</f>
         <v>33.333333333333336</v>
       </c>
     </row>
@@ -7668,7 +7691,7 @@
         <v>2</v>
       </c>
       <c r="O33">
-        <f t="shared" si="7"/>
+        <f>(N32-1)*100/$N$26</f>
         <v>22.222222222222221</v>
       </c>
     </row>
@@ -7683,7 +7706,7 @@
         <v>1</v>
       </c>
       <c r="O34">
-        <f t="shared" si="7"/>
+        <f>(N33-1)*100/$N$26</f>
         <v>11.111111111111111</v>
       </c>
     </row>
@@ -7698,7 +7721,7 @@
         <v>0</v>
       </c>
       <c r="O35">
-        <f t="shared" si="7"/>
+        <f>(N34-1)*100/$N$26</f>
         <v>0</v>
       </c>
     </row>
@@ -7710,672 +7733,694 @@
         <v>100</v>
       </c>
     </row>
-    <row r="37" spans="3:15" ht="18">
-      <c r="C37" s="48" t="s">
+    <row r="37" spans="3:15">
+      <c r="C37" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="D37" s="49"/>
-      <c r="E37" s="49"/>
-      <c r="F37" s="49"/>
-      <c r="G37" s="49"/>
-      <c r="H37" s="49"/>
-      <c r="I37" s="49"/>
-      <c r="J37" s="49"/>
-      <c r="K37" s="50"/>
-    </row>
-    <row r="38" spans="3:15" ht="18">
-      <c r="C38" s="47">
+      <c r="D37" s="48"/>
+      <c r="E37" s="48"/>
+      <c r="F37" s="48"/>
+      <c r="G37" s="48"/>
+      <c r="H37" s="48"/>
+      <c r="I37" s="48"/>
+      <c r="J37" s="48"/>
+      <c r="K37" s="49"/>
+    </row>
+    <row r="38" spans="3:15">
+      <c r="C38" s="46">
         <v>550</v>
       </c>
-      <c r="D38" s="47">
+      <c r="D38" s="46">
         <v>1.5</v>
       </c>
-      <c r="E38" s="47">
+      <c r="E38" s="46">
         <v>650</v>
       </c>
-      <c r="F38" s="47">
+      <c r="F38" s="46">
         <v>1.6</v>
       </c>
-      <c r="G38" s="47"/>
-      <c r="H38" s="47">
+      <c r="G38" s="46"/>
+      <c r="H38" s="46">
         <v>650</v>
       </c>
-      <c r="I38" s="47">
+      <c r="I38" s="46">
         <v>2.5</v>
       </c>
-      <c r="J38" s="47">
+      <c r="J38" s="46">
         <v>550</v>
       </c>
-      <c r="K38" s="47">
+      <c r="K38" s="46">
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="39" spans="3:15" ht="18">
-      <c r="C39" s="46">
+    <row r="39" spans="3:15">
+      <c r="C39" s="45">
         <v>550</v>
       </c>
-      <c r="D39" s="46">
+      <c r="D39" s="45">
         <v>1.6</v>
       </c>
-      <c r="E39" s="46">
+      <c r="E39" s="45">
         <v>650</v>
       </c>
-      <c r="F39" s="46">
+      <c r="F39" s="45">
         <v>1.65</v>
       </c>
-      <c r="G39" s="46"/>
-      <c r="H39" s="46">
+      <c r="G39" s="45"/>
+      <c r="H39" s="45">
         <v>650</v>
       </c>
-      <c r="I39" s="46">
+      <c r="I39" s="45">
         <v>2.2999999999999998</v>
       </c>
-      <c r="J39" s="46">
+      <c r="J39" s="45">
         <v>550</v>
       </c>
-      <c r="K39" s="46">
+      <c r="K39" s="45">
         <v>2.1</v>
       </c>
-    </row>
-    <row r="40" spans="3:15" ht="18">
-      <c r="C40" s="46">
+      <c r="N39" s="58"/>
+      <c r="O39" s="58"/>
+    </row>
+    <row r="40" spans="3:15">
+      <c r="C40" s="45">
         <v>550</v>
       </c>
-      <c r="D40" s="46">
+      <c r="D40" s="45">
         <v>1.65</v>
       </c>
-      <c r="E40" s="46">
+      <c r="E40" s="45">
         <v>650</v>
       </c>
-      <c r="F40" s="46">
+      <c r="F40" s="45">
         <v>1.8</v>
       </c>
-      <c r="G40" s="46"/>
-      <c r="H40" s="46">
+      <c r="G40" s="45"/>
+      <c r="H40" s="45">
         <v>650</v>
       </c>
-      <c r="I40" s="46">
+      <c r="I40" s="45">
         <v>2.1</v>
       </c>
-      <c r="J40" s="46">
+      <c r="J40" s="45">
         <v>550</v>
       </c>
-      <c r="K40" s="46">
+      <c r="K40" s="45">
         <v>2</v>
       </c>
-    </row>
-    <row r="41" spans="3:15" ht="18">
-      <c r="C41" s="46">
+      <c r="N40" s="58"/>
+      <c r="O40" s="58"/>
+    </row>
+    <row r="41" spans="3:15">
+      <c r="C41" s="45">
         <v>550</v>
       </c>
-      <c r="D41" s="46">
+      <c r="D41" s="45">
         <v>1.8</v>
       </c>
-      <c r="E41" s="46">
+      <c r="E41" s="45">
         <v>650</v>
       </c>
-      <c r="F41" s="46">
+      <c r="F41" s="45">
         <v>1.9</v>
       </c>
-      <c r="G41" s="46"/>
-      <c r="H41" s="46">
+      <c r="G41" s="45"/>
+      <c r="H41" s="45">
         <v>650</v>
       </c>
-      <c r="I41" s="46">
+      <c r="I41" s="45">
         <v>2</v>
       </c>
-      <c r="J41" s="46">
+      <c r="J41" s="45">
         <v>550</v>
       </c>
-      <c r="K41" s="46">
+      <c r="K41" s="45">
         <v>1.8</v>
       </c>
-    </row>
-    <row r="42" spans="3:15" ht="18">
-      <c r="C42" s="46">
+      <c r="N41" s="58"/>
+      <c r="O41" s="58"/>
+    </row>
+    <row r="42" spans="3:15">
+      <c r="C42" s="45">
         <v>550</v>
       </c>
-      <c r="D42" s="46">
+      <c r="D42" s="45">
         <v>1.9</v>
       </c>
-      <c r="E42" s="46">
+      <c r="E42" s="45">
         <v>650</v>
       </c>
-      <c r="F42" s="46">
+      <c r="F42" s="45">
         <v>2.1</v>
       </c>
-      <c r="G42" s="46"/>
-      <c r="H42" s="46">
+      <c r="G42" s="45"/>
+      <c r="H42" s="45">
         <v>650</v>
       </c>
-      <c r="I42" s="46">
+      <c r="I42" s="45">
         <v>1.8</v>
       </c>
-      <c r="J42" s="46">
+      <c r="J42" s="45">
         <v>550</v>
       </c>
-      <c r="K42" s="46">
+      <c r="K42" s="45">
         <v>1.7</v>
       </c>
-    </row>
-    <row r="43" spans="3:15" ht="18">
-      <c r="C43" s="46">
+      <c r="N42" s="58"/>
+      <c r="O42" s="58"/>
+    </row>
+    <row r="43" spans="3:15">
+      <c r="C43" s="45">
         <v>550</v>
       </c>
-      <c r="D43" s="46">
+      <c r="D43" s="45">
         <v>2.1</v>
       </c>
-      <c r="E43" s="46">
+      <c r="E43" s="45">
         <v>650</v>
       </c>
-      <c r="F43" s="46">
+      <c r="F43" s="45">
         <v>2.2999999999999998</v>
       </c>
-      <c r="G43" s="46"/>
-      <c r="H43" s="46">
+      <c r="G43" s="45"/>
+      <c r="H43" s="45">
         <v>650</v>
       </c>
-      <c r="I43" s="46">
+      <c r="I43" s="45">
         <v>1.7</v>
       </c>
-      <c r="J43" s="46">
+      <c r="J43" s="45">
         <v>550</v>
       </c>
-      <c r="K43" s="46">
+      <c r="K43" s="45">
         <v>1.6</v>
       </c>
-    </row>
-    <row r="44" spans="3:15" ht="18">
-      <c r="C44" s="51">
+      <c r="N43" s="58"/>
+      <c r="O43" s="58"/>
+    </row>
+    <row r="44" spans="3:15">
+      <c r="C44" s="50">
         <v>550</v>
       </c>
-      <c r="D44" s="51">
+      <c r="D44" s="50">
         <v>2.2999999999999998</v>
       </c>
-      <c r="E44" s="51">
+      <c r="E44" s="50">
         <v>650</v>
       </c>
-      <c r="F44" s="51">
+      <c r="F44" s="50">
         <v>2.4</v>
       </c>
-      <c r="G44" s="51"/>
-      <c r="H44" s="51">
+      <c r="G44" s="50"/>
+      <c r="H44" s="50">
         <v>650</v>
       </c>
-      <c r="I44" s="51">
+      <c r="I44" s="50">
         <v>1.6</v>
       </c>
-      <c r="J44" s="51">
+      <c r="J44" s="50">
         <v>550</v>
       </c>
-      <c r="K44" s="51">
+      <c r="K44" s="50">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="45" spans="3:15" ht="18">
-      <c r="C45" s="55"/>
-      <c r="D45" s="56"/>
-      <c r="E45" s="56"/>
-      <c r="F45" s="56"/>
-      <c r="G45" s="56"/>
-      <c r="H45" s="56"/>
-      <c r="I45" s="56"/>
-      <c r="J45" s="56"/>
-      <c r="K45" s="57"/>
-    </row>
-    <row r="46" spans="3:15" ht="18">
-      <c r="C46" s="52"/>
-      <c r="D46" s="53"/>
-      <c r="E46" s="53"/>
-      <c r="F46" s="53"/>
-      <c r="G46" s="53"/>
-      <c r="H46" s="53"/>
-      <c r="I46" s="53"/>
-      <c r="J46" s="53"/>
-      <c r="K46" s="54"/>
-    </row>
-    <row r="47" spans="3:15" ht="18">
-      <c r="C47" s="52" t="s">
+      <c r="N44" s="58"/>
+      <c r="O44" s="58"/>
+    </row>
+    <row r="45" spans="3:15">
+      <c r="C45" s="54"/>
+      <c r="D45" s="55"/>
+      <c r="E45" s="55"/>
+      <c r="F45" s="55"/>
+      <c r="G45" s="55"/>
+      <c r="H45" s="55"/>
+      <c r="I45" s="55"/>
+      <c r="J45" s="55"/>
+      <c r="K45" s="56"/>
+      <c r="N45" s="58"/>
+      <c r="O45" s="58"/>
+    </row>
+    <row r="46" spans="3:15">
+      <c r="C46" s="51"/>
+      <c r="D46" s="52"/>
+      <c r="E46" s="52"/>
+      <c r="F46" s="52"/>
+      <c r="G46" s="52"/>
+      <c r="H46" s="52"/>
+      <c r="I46" s="52"/>
+      <c r="J46" s="52"/>
+      <c r="K46" s="53"/>
+      <c r="N46" s="58"/>
+      <c r="O46" s="58"/>
+    </row>
+    <row r="47" spans="3:15">
+      <c r="C47" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="D47" s="53"/>
-      <c r="E47" s="53"/>
-      <c r="F47" s="53"/>
-      <c r="G47" s="53"/>
-      <c r="H47" s="53"/>
-      <c r="I47" s="53"/>
-      <c r="J47" s="53"/>
-      <c r="K47" s="54"/>
-    </row>
-    <row r="48" spans="3:15" ht="18">
-      <c r="C48" s="47">
-        <v>1</v>
-      </c>
-      <c r="D48" s="47">
+      <c r="D47" s="52"/>
+      <c r="E47" s="52"/>
+      <c r="F47" s="52"/>
+      <c r="G47" s="52"/>
+      <c r="H47" s="52"/>
+      <c r="I47" s="52"/>
+      <c r="J47" s="52"/>
+      <c r="K47" s="53"/>
+      <c r="N47" s="58"/>
+      <c r="O47" s="58"/>
+    </row>
+    <row r="48" spans="3:15">
+      <c r="C48" s="46">
+        <v>1</v>
+      </c>
+      <c r="D48" s="46">
         <v>300</v>
       </c>
-      <c r="E48" s="47">
+      <c r="E48" s="46">
         <v>2</v>
       </c>
-      <c r="F48" s="47">
+      <c r="F48" s="46">
         <v>400</v>
       </c>
-      <c r="G48" s="47">
+      <c r="G48" s="46">
         <v>2</v>
       </c>
-      <c r="H48" s="47">
+      <c r="H48" s="46">
         <v>450</v>
       </c>
-      <c r="I48" s="47">
-        <v>1</v>
-      </c>
-      <c r="J48" s="47">
+      <c r="I48" s="46">
+        <v>1</v>
+      </c>
+      <c r="J48" s="46">
         <v>300</v>
       </c>
-      <c r="K48" s="47"/>
-    </row>
-    <row r="49" spans="3:11" ht="18">
-      <c r="C49" s="46">
+      <c r="K48" s="46"/>
+      <c r="N48" s="58"/>
+      <c r="O48" s="58"/>
+    </row>
+    <row r="49" spans="3:15">
+      <c r="C49" s="45">
         <v>2</v>
       </c>
-      <c r="D49" s="46">
+      <c r="D49" s="45">
         <v>400</v>
       </c>
-      <c r="E49" s="46">
-        <v>3</v>
-      </c>
-      <c r="F49" s="46">
+      <c r="E49" s="45">
+        <v>3</v>
+      </c>
+      <c r="F49" s="45">
         <v>600</v>
       </c>
-      <c r="G49" s="46">
-        <v>3</v>
-      </c>
-      <c r="H49" s="46">
+      <c r="G49" s="45">
+        <v>3</v>
+      </c>
+      <c r="H49" s="45">
         <v>600</v>
       </c>
-      <c r="I49" s="46">
+      <c r="I49" s="45">
         <v>2</v>
       </c>
-      <c r="J49" s="46">
+      <c r="J49" s="45">
         <v>450</v>
       </c>
-      <c r="K49" s="46"/>
-    </row>
-    <row r="50" spans="3:11" ht="18">
-      <c r="C50" s="46">
-        <v>3</v>
-      </c>
-      <c r="D50" s="46">
+      <c r="K49" s="45"/>
+      <c r="N49" s="58"/>
+      <c r="O49" s="57"/>
+    </row>
+    <row r="50" spans="3:15">
+      <c r="C50" s="45">
+        <v>3</v>
+      </c>
+      <c r="D50" s="45">
         <v>600</v>
       </c>
-      <c r="E50" s="46">
+      <c r="E50" s="45">
         <v>4</v>
       </c>
-      <c r="F50" s="46">
+      <c r="F50" s="45">
         <v>900</v>
       </c>
-      <c r="G50" s="46">
+      <c r="G50" s="45">
         <v>4</v>
       </c>
-      <c r="H50" s="46">
+      <c r="H50" s="45">
         <v>1000</v>
       </c>
-      <c r="I50" s="46">
-        <v>3</v>
-      </c>
-      <c r="J50" s="46">
+      <c r="I50" s="45">
+        <v>3</v>
+      </c>
+      <c r="J50" s="45">
         <v>600</v>
       </c>
-      <c r="K50" s="46"/>
-    </row>
-    <row r="51" spans="3:11" ht="18">
-      <c r="C51" s="51">
+      <c r="K50" s="45"/>
+      <c r="N50" s="58"/>
+    </row>
+    <row r="51" spans="3:15">
+      <c r="C51" s="50">
         <v>4</v>
       </c>
-      <c r="D51" s="51">
+      <c r="D51" s="50">
         <v>900</v>
       </c>
-      <c r="E51" s="51">
-        <v>5</v>
-      </c>
-      <c r="F51" s="51">
+      <c r="E51" s="50">
+        <v>5</v>
+      </c>
+      <c r="F51" s="50">
         <v>1500</v>
       </c>
-      <c r="G51" s="51">
-        <v>5</v>
-      </c>
-      <c r="H51" s="51">
+      <c r="G51" s="50">
+        <v>5</v>
+      </c>
+      <c r="H51" s="50">
         <v>1500</v>
       </c>
-      <c r="I51" s="51">
+      <c r="I51" s="50">
         <v>4</v>
       </c>
-      <c r="J51" s="51">
+      <c r="J51" s="50">
         <v>1000</v>
       </c>
-      <c r="K51" s="51"/>
-    </row>
-    <row r="52" spans="3:11" ht="18">
-      <c r="C52" s="55"/>
-      <c r="D52" s="56"/>
-      <c r="E52" s="56"/>
-      <c r="F52" s="56"/>
-      <c r="G52" s="56"/>
-      <c r="H52" s="56"/>
-      <c r="I52" s="56"/>
-      <c r="J52" s="56"/>
-      <c r="K52" s="57"/>
-    </row>
-    <row r="53" spans="3:11" ht="18">
-      <c r="C53" s="52"/>
-      <c r="D53" s="53"/>
-      <c r="E53" s="53"/>
-      <c r="F53" s="53"/>
-      <c r="G53" s="53"/>
-      <c r="H53" s="53"/>
-      <c r="I53" s="53"/>
-      <c r="J53" s="53"/>
-      <c r="K53" s="54"/>
-    </row>
-    <row r="54" spans="3:11" ht="18">
-      <c r="C54" s="52" t="s">
+      <c r="K51" s="50"/>
+      <c r="N51" s="58"/>
+    </row>
+    <row r="52" spans="3:15">
+      <c r="C52" s="54"/>
+      <c r="D52" s="55"/>
+      <c r="E52" s="55"/>
+      <c r="F52" s="55"/>
+      <c r="G52" s="55"/>
+      <c r="H52" s="55"/>
+      <c r="I52" s="55"/>
+      <c r="J52" s="55"/>
+      <c r="K52" s="56"/>
+      <c r="N52" s="58"/>
+    </row>
+    <row r="53" spans="3:15">
+      <c r="C53" s="51"/>
+      <c r="D53" s="52"/>
+      <c r="E53" s="52"/>
+      <c r="F53" s="52"/>
+      <c r="G53" s="52"/>
+      <c r="H53" s="52"/>
+      <c r="I53" s="52"/>
+      <c r="J53" s="52"/>
+      <c r="K53" s="53"/>
+      <c r="N53" s="58"/>
+    </row>
+    <row r="54" spans="3:15">
+      <c r="C54" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="D54" s="53"/>
-      <c r="E54" s="53"/>
-      <c r="F54" s="53"/>
-      <c r="G54" s="53"/>
-      <c r="H54" s="53"/>
-      <c r="I54" s="53"/>
-      <c r="J54" s="53"/>
-      <c r="K54" s="54"/>
-    </row>
-    <row r="55" spans="3:11" ht="18">
-      <c r="C55" s="47">
-        <v>1</v>
-      </c>
-      <c r="D55" s="47">
+      <c r="D54" s="52"/>
+      <c r="E54" s="52"/>
+      <c r="F54" s="52"/>
+      <c r="G54" s="52"/>
+      <c r="H54" s="52"/>
+      <c r="I54" s="52"/>
+      <c r="J54" s="52"/>
+      <c r="K54" s="53"/>
+      <c r="N54" s="58"/>
+    </row>
+    <row r="55" spans="3:15">
+      <c r="C55" s="46">
+        <v>1</v>
+      </c>
+      <c r="D55" s="46">
         <v>200</v>
       </c>
-      <c r="E55" s="47">
+      <c r="E55" s="46">
         <v>2</v>
       </c>
-      <c r="F55" s="47">
+      <c r="F55" s="46">
         <v>300</v>
       </c>
-      <c r="G55" s="47">
+      <c r="G55" s="46">
         <v>2</v>
       </c>
-      <c r="H55" s="47">
+      <c r="H55" s="46">
         <v>400</v>
       </c>
-      <c r="I55" s="47">
-        <v>1</v>
-      </c>
-      <c r="J55" s="47">
+      <c r="I55" s="46">
+        <v>1</v>
+      </c>
+      <c r="J55" s="46">
         <v>300</v>
       </c>
-      <c r="K55" s="47"/>
-    </row>
-    <row r="56" spans="3:11" ht="18">
-      <c r="C56" s="46">
+      <c r="K55" s="46"/>
+      <c r="N55" s="58"/>
+    </row>
+    <row r="56" spans="3:15">
+      <c r="C56" s="45">
         <v>2</v>
       </c>
-      <c r="D56" s="46">
+      <c r="D56" s="45">
         <v>400</v>
       </c>
-      <c r="E56" s="46">
-        <v>3</v>
-      </c>
-      <c r="F56" s="46">
+      <c r="E56" s="45">
+        <v>3</v>
+      </c>
+      <c r="F56" s="45">
         <v>500</v>
       </c>
-      <c r="G56" s="46">
-        <v>3</v>
-      </c>
-      <c r="H56" s="46">
+      <c r="G56" s="45">
+        <v>3</v>
+      </c>
+      <c r="H56" s="45">
         <v>700</v>
       </c>
-      <c r="I56" s="46">
+      <c r="I56" s="45">
         <v>2</v>
       </c>
-      <c r="J56" s="46">
+      <c r="J56" s="45">
         <v>400</v>
       </c>
-      <c r="K56" s="46"/>
-    </row>
-    <row r="57" spans="3:11" ht="18">
-      <c r="C57" s="46">
-        <v>3</v>
-      </c>
-      <c r="D57" s="46">
+      <c r="K56" s="45"/>
+      <c r="N56" s="58"/>
+    </row>
+    <row r="57" spans="3:15">
+      <c r="C57" s="45">
+        <v>3</v>
+      </c>
+      <c r="D57" s="45">
         <v>500</v>
       </c>
-      <c r="E57" s="46">
+      <c r="E57" s="45">
         <v>4</v>
       </c>
-      <c r="F57" s="46">
+      <c r="F57" s="45">
         <v>600</v>
       </c>
-      <c r="G57" s="46">
+      <c r="G57" s="45">
         <v>4</v>
       </c>
-      <c r="H57" s="46">
+      <c r="H57" s="45">
         <v>900</v>
       </c>
-      <c r="I57" s="46">
-        <v>3</v>
-      </c>
-      <c r="J57" s="46">
+      <c r="I57" s="45">
+        <v>3</v>
+      </c>
+      <c r="J57" s="45">
         <v>700</v>
       </c>
-      <c r="K57" s="46"/>
-    </row>
-    <row r="58" spans="3:11" ht="18">
-      <c r="C58" s="51">
+      <c r="K57" s="45"/>
+    </row>
+    <row r="58" spans="3:15">
+      <c r="C58" s="50">
         <v>4</v>
       </c>
-      <c r="D58" s="51">
+      <c r="D58" s="50">
         <v>600</v>
       </c>
-      <c r="E58" s="51">
-        <v>5</v>
-      </c>
-      <c r="F58" s="51">
+      <c r="E58" s="50">
+        <v>5</v>
+      </c>
+      <c r="F58" s="50">
         <v>1500</v>
       </c>
-      <c r="G58" s="51">
-        <v>5</v>
-      </c>
-      <c r="H58" s="51">
+      <c r="G58" s="50">
+        <v>5</v>
+      </c>
+      <c r="H58" s="50">
         <v>1500</v>
       </c>
-      <c r="I58" s="51">
+      <c r="I58" s="50">
         <v>4</v>
       </c>
-      <c r="J58" s="51">
+      <c r="J58" s="50">
         <v>900</v>
       </c>
-      <c r="K58" s="51"/>
-    </row>
-    <row r="59" spans="3:11" ht="18">
-      <c r="C59" s="55"/>
-      <c r="D59" s="56"/>
-      <c r="E59" s="56"/>
-      <c r="F59" s="56"/>
-      <c r="G59" s="56"/>
-      <c r="H59" s="56"/>
-      <c r="I59" s="56"/>
-      <c r="J59" s="56"/>
-      <c r="K59" s="57"/>
-    </row>
-    <row r="60" spans="3:11" ht="18">
-      <c r="C60" s="52"/>
-      <c r="D60" s="53"/>
-      <c r="E60" s="53"/>
-      <c r="F60" s="53"/>
-      <c r="G60" s="53"/>
-      <c r="H60" s="53"/>
-      <c r="I60" s="53"/>
-      <c r="J60" s="53"/>
-      <c r="K60" s="54"/>
-    </row>
-    <row r="61" spans="3:11" ht="18">
-      <c r="C61" s="52" t="s">
+      <c r="K58" s="50"/>
+    </row>
+    <row r="59" spans="3:15">
+      <c r="C59" s="54"/>
+      <c r="D59" s="55"/>
+      <c r="E59" s="55"/>
+      <c r="F59" s="55"/>
+      <c r="G59" s="55"/>
+      <c r="H59" s="55"/>
+      <c r="I59" s="55"/>
+      <c r="J59" s="55"/>
+      <c r="K59" s="56"/>
+    </row>
+    <row r="60" spans="3:15">
+      <c r="C60" s="51"/>
+      <c r="D60" s="52"/>
+      <c r="E60" s="52"/>
+      <c r="F60" s="52"/>
+      <c r="G60" s="52"/>
+      <c r="H60" s="52"/>
+      <c r="I60" s="52"/>
+      <c r="J60" s="52"/>
+      <c r="K60" s="53"/>
+    </row>
+    <row r="61" spans="3:15">
+      <c r="C61" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="D61" s="53"/>
-      <c r="E61" s="53"/>
-      <c r="F61" s="53"/>
-      <c r="G61" s="53"/>
-      <c r="H61" s="53"/>
-      <c r="I61" s="53"/>
-      <c r="J61" s="53"/>
-      <c r="K61" s="54"/>
-    </row>
-    <row r="62" spans="3:11" ht="18">
-      <c r="C62" s="47">
-        <v>1</v>
-      </c>
-      <c r="D62" s="47">
+      <c r="D61" s="52"/>
+      <c r="E61" s="52"/>
+      <c r="F61" s="52"/>
+      <c r="G61" s="52"/>
+      <c r="H61" s="52"/>
+      <c r="I61" s="52"/>
+      <c r="J61" s="52"/>
+      <c r="K61" s="53"/>
+    </row>
+    <row r="62" spans="3:15">
+      <c r="C62" s="46">
+        <v>1</v>
+      </c>
+      <c r="D62" s="46">
         <v>300</v>
       </c>
-      <c r="E62" s="47">
+      <c r="E62" s="46">
         <v>2</v>
       </c>
-      <c r="F62" s="47">
+      <c r="F62" s="46">
         <v>400</v>
       </c>
-      <c r="G62" s="47">
+      <c r="G62" s="46">
         <v>2</v>
       </c>
-      <c r="H62" s="47">
+      <c r="H62" s="46">
         <v>400</v>
       </c>
-      <c r="I62" s="47">
-        <v>1</v>
-      </c>
-      <c r="J62" s="47">
+      <c r="I62" s="46">
+        <v>1</v>
+      </c>
+      <c r="J62" s="46">
         <v>300</v>
       </c>
-      <c r="K62" s="47"/>
-    </row>
-    <row r="63" spans="3:11" ht="18">
-      <c r="C63" s="46">
+      <c r="K62" s="46"/>
+    </row>
+    <row r="63" spans="3:15">
+      <c r="C63" s="45">
         <v>2</v>
       </c>
-      <c r="D63" s="46">
+      <c r="D63" s="45">
         <v>400</v>
       </c>
-      <c r="E63" s="46">
-        <v>3</v>
-      </c>
-      <c r="F63" s="46">
+      <c r="E63" s="45">
+        <v>3</v>
+      </c>
+      <c r="F63" s="45">
         <v>500</v>
       </c>
-      <c r="G63" s="46">
-        <v>3</v>
-      </c>
-      <c r="H63" s="46">
+      <c r="G63" s="45">
+        <v>3</v>
+      </c>
+      <c r="H63" s="45">
         <v>600</v>
       </c>
-      <c r="I63" s="46">
+      <c r="I63" s="45">
         <v>2</v>
       </c>
-      <c r="J63" s="46">
+      <c r="J63" s="45">
         <v>400</v>
       </c>
-      <c r="K63" s="46"/>
-    </row>
-    <row r="64" spans="3:11" ht="18">
-      <c r="C64" s="46">
-        <v>3</v>
-      </c>
-      <c r="D64" s="46">
+      <c r="K63" s="45"/>
+    </row>
+    <row r="64" spans="3:15">
+      <c r="C64" s="45">
+        <v>3</v>
+      </c>
+      <c r="D64" s="45">
         <v>500</v>
       </c>
-      <c r="E64" s="46">
+      <c r="E64" s="45">
         <v>4</v>
       </c>
-      <c r="F64" s="46">
+      <c r="F64" s="45">
         <v>1000</v>
       </c>
-      <c r="G64" s="46">
+      <c r="G64" s="45">
         <v>4</v>
       </c>
-      <c r="H64" s="46">
+      <c r="H64" s="45">
         <v>900</v>
       </c>
-      <c r="I64" s="46">
-        <v>3</v>
-      </c>
-      <c r="J64" s="46">
+      <c r="I64" s="45">
+        <v>3</v>
+      </c>
+      <c r="J64" s="45">
         <v>600</v>
       </c>
-      <c r="K64" s="46"/>
-    </row>
-    <row r="65" spans="3:11" ht="18">
-      <c r="C65" s="46">
+      <c r="K64" s="45"/>
+    </row>
+    <row r="65" spans="3:11">
+      <c r="C65" s="45">
         <v>4</v>
       </c>
-      <c r="D65" s="46">
+      <c r="D65" s="45">
         <v>1000</v>
       </c>
-      <c r="E65" s="46">
-        <v>5</v>
-      </c>
-      <c r="F65" s="46">
+      <c r="E65" s="45">
+        <v>5</v>
+      </c>
+      <c r="F65" s="45">
         <v>1500</v>
       </c>
-      <c r="G65" s="46">
-        <v>5</v>
-      </c>
-      <c r="H65" s="46">
+      <c r="G65" s="45">
+        <v>5</v>
+      </c>
+      <c r="H65" s="45">
         <v>1500</v>
       </c>
-      <c r="I65" s="46">
+      <c r="I65" s="45">
         <v>4</v>
       </c>
-      <c r="J65" s="46">
+      <c r="J65" s="45">
         <v>900</v>
       </c>
-      <c r="K65" s="46"/>
+      <c r="K65" s="45"/>
     </row>
     <row r="66" spans="3:11">
-      <c r="G66" s="45"/>
-      <c r="H66" s="45"/>
+      <c r="G66"/>
     </row>
     <row r="67" spans="3:11">
-      <c r="G67" s="45"/>
-      <c r="H67" s="45"/>
+      <c r="G67"/>
     </row>
     <row r="68" spans="3:11">
-      <c r="G68" s="45"/>
-      <c r="H68" s="45"/>
+      <c r="G68"/>
     </row>
     <row r="69" spans="3:11">
-      <c r="G69" s="45"/>
-      <c r="H69" s="45"/>
+      <c r="G69"/>
     </row>
     <row r="70" spans="3:11">
-      <c r="G70" s="45"/>
-      <c r="H70" s="45"/>
+      <c r="G70"/>
     </row>
     <row r="71" spans="3:11">
-      <c r="G71" s="45"/>
-      <c r="H71" s="45"/>
+      <c r="G71"/>
     </row>
     <row r="72" spans="3:11">
-      <c r="G72" s="45"/>
-      <c r="H72" s="45"/>
+      <c r="G72"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="K25:K36">
-    <sortCondition ref="K25:K36"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="N39:N50">
+    <sortCondition descending="1" ref="N39:N50"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -8383,13 +8428,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{863C0C67-8C9F-2A4E-AC76-F4E9B1B5F2AD}">
   <dimension ref="A1:V27"/>
   <sheetViews>
-    <sheetView zoomScale="88" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView zoomScale="56" workbookViewId="0">
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6"/>
   <cols>
-    <col min="13" max="13" width="39.33203125" style="28" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="39.296875" style="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22">
@@ -8999,7 +9044,7 @@
     <row r="13" spans="1:22">
       <c r="G13" s="9"/>
     </row>
-    <row r="14" spans="1:22" ht="17" thickBot="1">
+    <row r="14" spans="1:22" ht="16.2" thickBot="1">
       <c r="G14" s="9"/>
     </row>
     <row r="15" spans="1:22" s="14" customFormat="1">
@@ -9461,6 +9506,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -9468,13 +9514,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93F1BF91-8CAF-244E-B6BF-FE8B646402AF}">
   <dimension ref="A1:AB49"/>
   <sheetViews>
-    <sheetView zoomScale="82" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView zoomScale="64" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6"/>
   <cols>
-    <col min="13" max="13" width="10.83203125" style="28"/>
+    <col min="13" max="13" width="10.796875" style="28"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28">
@@ -10221,7 +10267,7 @@
       <c r="AA13" s="23"/>
       <c r="AB13" s="23"/>
     </row>
-    <row r="14" spans="1:28" ht="17" thickBot="1">
+    <row r="14" spans="1:28" ht="16.2" thickBot="1">
       <c r="A14" s="23"/>
       <c r="B14" s="23"/>
       <c r="C14" s="23"/>
@@ -10369,7 +10415,7 @@
       <c r="AA17" s="23"/>
       <c r="AB17" s="23"/>
     </row>
-    <row r="18" spans="1:28" ht="17" thickBot="1">
+    <row r="18" spans="1:28" ht="16.2" thickBot="1">
       <c r="A18" s="23"/>
       <c r="B18" s="23"/>
       <c r="C18" s="23"/>
@@ -11613,18 +11659,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4473C636-8F8B-734A-9EFB-C73EEF4CFCCF}">
   <dimension ref="A1:AB30"/>
   <sheetViews>
-    <sheetView zoomScale="113" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="56" workbookViewId="0">
+      <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6"/>
   <cols>
     <col min="2" max="2" width="47" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" customWidth="1"/>
-    <col min="13" max="13" width="39.33203125" style="28" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.69921875" customWidth="1"/>
+    <col min="13" max="13" width="39.296875" style="28" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="2.83203125" customWidth="1"/>
-    <col min="24" max="24" width="10.83203125" style="28"/>
+    <col min="23" max="23" width="2.796875" customWidth="1"/>
+    <col min="24" max="24" width="10.796875" style="28"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24">
@@ -12293,7 +12339,7 @@
       <c r="U13" s="23"/>
       <c r="V13" s="23"/>
     </row>
-    <row r="14" spans="1:24" ht="17" thickBot="1">
+    <row r="14" spans="1:24" ht="16.2" thickBot="1">
       <c r="A14" s="23"/>
       <c r="B14" s="23"/>
       <c r="C14" s="23"/>
@@ -12317,7 +12363,7 @@
       <c r="U14" s="23"/>
       <c r="V14" s="23"/>
     </row>
-    <row r="15" spans="1:24" s="19" customFormat="1" ht="17" thickBot="1">
+    <row r="15" spans="1:24" s="19" customFormat="1" ht="16.2" thickBot="1">
       <c r="A15" s="35"/>
       <c r="B15" s="35" t="s">
         <v>26</v>
@@ -12639,7 +12685,7 @@
         <v>-1</v>
       </c>
       <c r="AB21">
-        <f t="shared" si="2"/>
+        <f>RANK(AA21,_xlfn.ANCHORARRAY($AA$19),0)</f>
         <v>5</v>
       </c>
     </row>
@@ -13039,7 +13085,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="2:28" ht="17" thickBot="1"/>
+    <row r="28" spans="2:28" ht="16.2" thickBot="1"/>
     <row r="29" spans="2:28" s="14" customFormat="1">
       <c r="M29" s="29" t="s">
         <v>33</v>

</xml_diff>

<commit_message>
correction excel erreur utilité additive et powerpoint
</commit_message>
<xml_diff>
--- a/Café.xlsx
+++ b/Café.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ingri\Ma1\AMCD\projetaidmulticrit\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noafoucoux/Documents/Cours/ma2/aidmulticrit/projetaidmulticrit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68EE0E71-74D3-42A5-ABAB-1E3AB9235540}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE668DAC-8FCC-444A-BDDC-F3F333249753}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="4" xr2:uid="{E16892A5-2733-6247-BC2F-556276338AEC}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="4" xr2:uid="{E16892A5-2733-6247-BC2F-556276338AEC}"/>
   </bookViews>
   <sheets>
     <sheet name="Dominance" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -181,13 +181,13 @@
     <t>=&gt; PQ ? Car on veut avoir 0,3 et 0,3 absolument et soit mousse et température ou capacité du reservoir'</t>
   </si>
   <si>
-    <t>poids</t>
+    <t>Utilité Additive</t>
   </si>
   <si>
-    <t>Normalisat°</t>
+    <t>Poids</t>
   </si>
   <si>
-    <t>Utilité Additive</t>
+    <t>norm</t>
   </si>
 </sst>
 </file>
@@ -253,6 +253,7 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Helvetica"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -577,7 +578,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -635,11 +636,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2093,31 +2092,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>70.899645951661682</c:v>
+                  <c:v>80.943165541912734</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>50.73981964406417</c:v>
+                  <c:v>58.206898468528273</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>55.3488698183574</c:v>
+                  <c:v>63.019483297095071</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42.365634935252615</c:v>
+                  <c:v>54.517203308102289</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>41.246390548778066</c:v>
+                  <c:v>59.941071576942505</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>63.702909919003439</c:v>
+                  <c:v>41.71687419363937</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>41.246390548778066</c:v>
+                  <c:v>59.061525371184644</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>60.11461062517499</c:v>
+                  <c:v>67.899497655980042</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.6291947824587503</c:v>
+                  <c:v>36.841258738511456</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5575,14 +5574,11 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="9" max="9" width="24" customWidth="1"/>
-    <col min="10" max="10" width="14.796875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.19921875" customWidth="1"/>
-    <col min="12" max="12" width="15.09765625" customWidth="1"/>
-    <col min="13" max="15" width="15.19921875" customWidth="1"/>
-    <col min="16" max="18" width="15.09765625" customWidth="1"/>
+    <col min="10" max="10" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="18" width="15.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24">
@@ -6602,25 +6598,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41137E64-42F2-044D-BD17-AF19D2ABB3C0}">
   <dimension ref="A1:O72"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="67" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView zoomScaleNormal="67" workbookViewId="0">
+      <selection activeCell="J39" sqref="J39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="2" max="2" width="43.19921875" customWidth="1"/>
-    <col min="3" max="3" width="17.796875" customWidth="1"/>
-    <col min="4" max="5" width="13.69921875" customWidth="1"/>
-    <col min="6" max="6" width="11.296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.8984375" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="11.296875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.796875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.296875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.8984375" style="28" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="11.296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.1640625" customWidth="1"/>
+    <col min="3" max="3" width="17.83203125" customWidth="1"/>
+    <col min="4" max="5" width="13.6640625" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.83203125" style="28" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:14">
       <c r="C1" t="s">
         <v>11</v>
       </c>
@@ -6652,14 +6648,13 @@
         <v>9</v>
       </c>
       <c r="M1" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="N1" s="61" t="s">
+        <v>39</v>
+      </c>
+      <c r="N1" t="s">
         <v>31</v>
       </c>
-      <c r="O1" s="61"/>
-    </row>
-    <row r="2" spans="1:15">
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -6698,18 +6693,19 @@
         <v>-2.8421709430404007E-14</v>
       </c>
       <c r="L2">
-        <f t="shared" ref="L2:L18" ca="1" si="3">_xlfn.FORECAST.LINEAR(G2,OFFSET(L$26:L$27,MATCH(G2,G$26:G$27,1)-1,0,2),OFFSET(G$26:G$27,MATCH(G2,G$26:G$27,1)-1,0,2))</f>
+        <f t="shared" ref="L2:L10" ca="1" si="3">_xlfn.FORECAST.LINEAR(G2,OFFSET(L$26:L$27,MATCH(G2,G$26:G$27,1)-1,0,2),OFFSET(G$26:G$27,MATCH(G2,G$26:G$27,1)-1,0,2))</f>
         <v>100</v>
       </c>
-      <c r="M2" s="28">
-        <v>70.899645951661682</v>
+      <c r="M2" s="28" cm="1">
+        <f t="array" aca="1" ref="M2" ca="1">MMULT(H2:L2,TRANSPOSE(H$19:L$19))</f>
+        <v>80.943165541912734</v>
       </c>
       <c r="N2">
-        <f>RANK(M2,M$2:M$10)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15">
+        <f ca="1">RANK(M2,M$2:M$10)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -6751,15 +6747,16 @@
         <f t="shared" ca="1" si="3"/>
         <v>72.375127420998979</v>
       </c>
-      <c r="M3" s="28">
-        <v>50.73981964406417</v>
+      <c r="M3" s="28" cm="1">
+        <f t="array" aca="1" ref="M3" ca="1">MMULT(H3:L3,TRANSPOSE(H$19:L$19))</f>
+        <v>58.206898468528273</v>
       </c>
       <c r="N3">
-        <f t="shared" ref="N3:N10" si="5">RANK(M3,M$2:M$10)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15">
+        <f t="shared" ref="N3:N10" ca="1" si="5">RANK(M3,M$2:M$10)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -6801,15 +6798,16 @@
         <f t="shared" ca="1" si="3"/>
         <v>77.573904179408771</v>
       </c>
-      <c r="M4" s="28">
-        <v>55.3488698183574</v>
+      <c r="M4" s="28" cm="1">
+        <f t="array" aca="1" ref="M4" ca="1">MMULT(H4:L4,TRANSPOSE(H$19:L$19))</f>
+        <v>63.019483297095071</v>
       </c>
       <c r="N4">
-        <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15">
+        <f t="shared" ca="1" si="5"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -6851,15 +6849,16 @@
         <f t="shared" ca="1" si="3"/>
         <v>77.573904179408771</v>
       </c>
-      <c r="M5" s="28">
-        <v>42.365634935252615</v>
+      <c r="M5" s="28" cm="1">
+        <f t="array" aca="1" ref="M5" ca="1">MMULT(H5:L5,TRANSPOSE(H$19:L$19))</f>
+        <v>54.517203308102289</v>
       </c>
       <c r="N5">
-        <f t="shared" si="5"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15">
+        <f t="shared" ca="1" si="5"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -6898,18 +6897,19 @@
         <v>44.444444444444429</v>
       </c>
       <c r="L6">
-        <f t="shared" ca="1" si="3"/>
+        <f ca="1">_xlfn.FORECAST.LINEAR(G6,OFFSET(L$26:L$27,MATCH(G6,G$26:G$27,1)-1,0,2),OFFSET(G$26:G$27,MATCH(G6,G$26:G$27,1)-1,0,2))</f>
         <v>95.412844036697251</v>
       </c>
-      <c r="M6" s="28">
-        <v>41.246390548778066</v>
+      <c r="M6" s="28" cm="1">
+        <f t="array" aca="1" ref="M6" ca="1">MMULT(H6:L6,TRANSPOSE(H$19:L$19))</f>
+        <v>59.941071576942505</v>
       </c>
       <c r="N6">
-        <f t="shared" si="5"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15">
+        <f t="shared" ca="1" si="5"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -6951,15 +6951,16 @@
         <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
-      <c r="M7" s="28">
-        <v>63.702909919003439</v>
+      <c r="M7" s="28" cm="1">
+        <f t="array" aca="1" ref="M7" ca="1">MMULT(H7:L7,TRANSPOSE(H$19:L$19))</f>
+        <v>41.71687419363937</v>
       </c>
       <c r="N7">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15">
+        <f t="shared" ca="1" si="5"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -7001,15 +7002,16 @@
         <f t="shared" ca="1" si="3"/>
         <v>92.864424057084619</v>
       </c>
-      <c r="M8" s="28">
-        <v>41.246390548778066</v>
+      <c r="M8" s="28" cm="1">
+        <f t="array" aca="1" ref="M8" ca="1">MMULT(H8:L8,TRANSPOSE(H$19:L$19))</f>
+        <v>59.061525371184644</v>
       </c>
       <c r="N8">
-        <f t="shared" si="5"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15">
+        <f t="shared" ca="1" si="5"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -7051,15 +7053,16 @@
         <f ca="1">_xlfn.FORECAST.LINEAR(G9,OFFSET(L$26:L$27,MATCH(G9,G$26:G$27,1)-1,0,2),OFFSET(G$26:G$27,MATCH(G9,G$26:G$27,1)-1,0,2))</f>
         <v>82.670744138634049</v>
       </c>
-      <c r="M9" s="28">
-        <v>60.11461062517499</v>
+      <c r="M9" s="28" cm="1">
+        <f t="array" aca="1" ref="M9" ca="1">MMULT(H9:L9,TRANSPOSE(H$19:L$19))</f>
+        <v>67.899497655980042</v>
       </c>
       <c r="N9">
-        <f t="shared" si="5"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" ht="16.2" thickBot="1">
+        <f t="shared" ca="1" si="5"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="17" thickBot="1">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -7101,15 +7104,16 @@
         <f t="shared" ca="1" si="3"/>
         <v>97.961264016309883</v>
       </c>
-      <c r="M10" s="28">
-        <v>4.6291947824587503</v>
+      <c r="M10" s="28" cm="1">
+        <f t="array" aca="1" ref="M10" ca="1">MMULT(H10:L10,TRANSPOSE(H$19:L$19))</f>
+        <v>36.841258738511456</v>
       </c>
       <c r="N10">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:15" s="14" customFormat="1">
+    <row r="11" spans="1:14" s="14" customFormat="1">
       <c r="A11" s="12"/>
       <c r="B11" s="12"/>
       <c r="C11" s="15"/>
@@ -7129,12 +7133,12 @@
         <v>-2.8421709430404007E-14</v>
       </c>
       <c r="L11" s="14">
-        <f t="shared" ca="1" si="3"/>
+        <f ca="1">_xlfn.FORECAST.LINEAR(G11,OFFSET(L$26:L$27,MATCH(G11,G$26:G$27,1)-1,0,2),OFFSET(G$26:G$27,MATCH(G11,G$26:G$27,1)-1,0,2))</f>
         <v>77.471967380224271</v>
       </c>
       <c r="M11" s="29"/>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:14">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="16"/>
@@ -7154,11 +7158,11 @@
         <v>11.111111111111086</v>
       </c>
       <c r="L12">
-        <f t="shared" ca="1" si="3"/>
+        <f ca="1">_xlfn.FORECAST.LINEAR(G12,OFFSET(L$26:L$27,MATCH(G12,G$26:G$27,1)-1,0,2),OFFSET(G$26:G$27,MATCH(G12,G$26:G$27,1)-1,0,2))</f>
         <v>67.278287461773701</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:14">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="16"/>
@@ -7178,11 +7182,11 @@
       </c>
       <c r="K13" s="17"/>
       <c r="L13">
-        <f t="shared" ca="1" si="3"/>
+        <f ca="1">_xlfn.FORECAST.LINEAR(G13,OFFSET(L$26:L$27,MATCH(G13,G$26:G$27,1)-1,0,2),OFFSET(G$26:G$27,MATCH(G13,G$26:G$27,1)-1,0,2))</f>
         <v>92.762487257900105</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:14">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="16"/>
@@ -7202,11 +7206,11 @@
       </c>
       <c r="K14" s="17"/>
       <c r="L14">
-        <f t="shared" ca="1" si="3"/>
+        <f ca="1">_xlfn.FORECAST.LINEAR(G14,OFFSET(L$26:L$27,MATCH(G14,G$26:G$27,1)-1,0,2),OFFSET(G$26:G$27,MATCH(G14,G$26:G$27,1)-1,0,2))</f>
         <v>82.568807339449535</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:14">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="16"/>
@@ -7226,11 +7230,11 @@
       <c r="J15" s="17"/>
       <c r="K15" s="17"/>
       <c r="L15">
-        <f t="shared" ca="1" si="3"/>
+        <f ca="1">_xlfn.FORECAST.LINEAR(G15,OFFSET(L$26:L$27,MATCH(G15,G$26:G$27,1)-1,0,2),OFFSET(G$26:G$27,MATCH(G15,G$26:G$27,1)-1,0,2))</f>
         <v>92.762487257900105</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:14">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="16"/>
@@ -7250,7 +7254,7 @@
       <c r="J16" s="17"/>
       <c r="K16" s="17"/>
       <c r="L16">
-        <f t="shared" ca="1" si="3"/>
+        <f ca="1">_xlfn.FORECAST.LINEAR(G16,OFFSET(L$26:L$27,MATCH(G16,G$26:G$27,1)-1,0,2),OFFSET(G$26:G$27,MATCH(G16,G$26:G$27,1)-1,0,2))</f>
         <v>82.568807339449535</v>
       </c>
     </row>
@@ -7274,11 +7278,11 @@
       <c r="J17" s="17"/>
       <c r="K17" s="17"/>
       <c r="L17">
-        <f t="shared" ca="1" si="3"/>
+        <f ca="1">_xlfn.FORECAST.LINEAR(G17,OFFSET(L$26:L$27,MATCH(G17,G$26:G$27,1)-1,0,2),OFFSET(G$26:G$27,MATCH(G17,G$26:G$27,1)-1,0,2))</f>
         <v>92.762487257900105</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="16.2" thickBot="1">
+    <row r="18" spans="1:15" ht="17" thickBot="1">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1">
@@ -7298,7 +7302,7 @@
       <c r="J18" s="17"/>
       <c r="K18" s="17"/>
       <c r="L18">
-        <f t="shared" ca="1" si="3"/>
+        <f ca="1">_xlfn.FORECAST.LINEAR(G18,OFFSET(L$26:L$27,MATCH(G18,G$26:G$27,1)-1,0,2),OFFSET(G$26:G$27,MATCH(G18,G$26:G$27,1)-1,0,2))</f>
         <v>72.375127420998979</v>
       </c>
     </row>
@@ -7309,56 +7313,56 @@
       <c r="D19" s="12"/>
       <c r="E19" s="12"/>
       <c r="F19" s="12"/>
-      <c r="G19" s="60" t="s">
+      <c r="G19" s="59" t="s">
         <v>40</v>
       </c>
       <c r="H19" s="14">
         <f ca="1">H20/SUM($H20:$L20)</f>
-        <v>0.17907910183592804</v>
+        <v>0.11727282743438314</v>
       </c>
       <c r="I19" s="14">
-        <f t="shared" ref="I19:L19" ca="1" si="6">I20/SUM($H20:$L20)</f>
-        <v>6.7154663188473074E-2</v>
+        <f t="shared" ref="I19:K19" ca="1" si="6">I20/SUM($H20:$L20)</f>
+        <v>4.3977310287893707E-2</v>
       </c>
       <c r="J19" s="14">
         <f t="shared" ca="1" si="6"/>
-        <v>0.77552434584866403</v>
+        <v>0.50786457967161114</v>
       </c>
       <c r="K19" s="14">
         <f t="shared" ca="1" si="6"/>
-        <v>0.24175678747850296</v>
+        <v>0.1583183170364173</v>
       </c>
       <c r="L19" s="14">
-        <f t="shared" ca="1" si="6"/>
-        <v>-0.26351489835156805</v>
+        <f ca="1">L20/SUM($H20:$L20)</f>
+        <v>0.17256696556969475</v>
       </c>
       <c r="M19" s="29"/>
     </row>
     <row r="20" spans="1:15">
-      <c r="G20" s="59" t="s">
-        <v>39</v>
+      <c r="G20" s="58" t="s">
+        <v>41</v>
       </c>
       <c r="H20">
-        <f ca="1">(L17-L18)/(H17-H18)</f>
-        <v>-0.67957866123003752</v>
+        <f ca="1">(L17-L18)/(H18-H17)</f>
+        <v>0.67957866123003752</v>
       </c>
       <c r="I20">
-        <f ca="1">(L15-L16)/(I15-I16)</f>
-        <v>-0.25484199796126428</v>
+        <f ca="1">(L15-L16)/(I16-I15)</f>
+        <v>0.25484199796126428</v>
       </c>
       <c r="J20">
-        <f ca="1">(J13-J14)/(L13-L14)</f>
-        <v>-2.9429999999999974</v>
+        <f ca="1">(J13-J14)/(L14-L13)</f>
+        <v>2.9429999999999974</v>
       </c>
       <c r="K20">
-        <f ca="1">(L11-L12)/(K11-K12)</f>
-        <v>-0.91743119266055106</v>
+        <f ca="1">(L11-L12)/(K12-K11)</f>
+        <v>0.91743119266055106</v>
       </c>
       <c r="L20">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:15" s="20" customFormat="1" ht="16.2" thickBot="1">
+    <row r="21" spans="1:15" s="20" customFormat="1" ht="17" thickBot="1">
       <c r="G21" s="21"/>
       <c r="M21" s="40"/>
     </row>
@@ -7484,7 +7488,7 @@
         <v>9</v>
       </c>
       <c r="O26">
-        <f>(N25-1)*100/$N$26</f>
+        <f t="shared" ref="O26:O35" si="7">(N25-1)*100/$N$26</f>
         <v>100</v>
       </c>
     </row>
@@ -7523,7 +7527,7 @@
         <v>8</v>
       </c>
       <c r="O27">
-        <f>(N26-1)*100/$N$26</f>
+        <f t="shared" si="7"/>
         <v>88.888888888888886</v>
       </c>
     </row>
@@ -7562,7 +7566,7 @@
         <v>7</v>
       </c>
       <c r="O28">
-        <f>(N27-1)*100/$N$26</f>
+        <f t="shared" si="7"/>
         <v>77.777777777777771</v>
       </c>
     </row>
@@ -7595,7 +7599,7 @@
         <v>6</v>
       </c>
       <c r="O29">
-        <f>(N28-1)*100/$N$26</f>
+        <f t="shared" si="7"/>
         <v>66.666666666666671</v>
       </c>
     </row>
@@ -7628,7 +7632,7 @@
         <v>5</v>
       </c>
       <c r="O30">
-        <f>(N29-1)*100/$N$26</f>
+        <f t="shared" si="7"/>
         <v>55.555555555555557</v>
       </c>
     </row>
@@ -7661,7 +7665,7 @@
         <v>4</v>
       </c>
       <c r="O31">
-        <f>(N30-1)*100/$N$26</f>
+        <f t="shared" si="7"/>
         <v>44.444444444444443</v>
       </c>
     </row>
@@ -7676,7 +7680,7 @@
         <v>3</v>
       </c>
       <c r="O32">
-        <f>(N31-1)*100/$N$26</f>
+        <f t="shared" si="7"/>
         <v>33.333333333333336</v>
       </c>
     </row>
@@ -7691,7 +7695,7 @@
         <v>2</v>
       </c>
       <c r="O33">
-        <f>(N32-1)*100/$N$26</f>
+        <f t="shared" si="7"/>
         <v>22.222222222222221</v>
       </c>
     </row>
@@ -7706,7 +7710,7 @@
         <v>1</v>
       </c>
       <c r="O34">
-        <f>(N33-1)*100/$N$26</f>
+        <f t="shared" si="7"/>
         <v>11.111111111111111</v>
       </c>
     </row>
@@ -7721,7 +7725,7 @@
         <v>0</v>
       </c>
       <c r="O35">
-        <f>(N34-1)*100/$N$26</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -7733,7 +7737,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="37" spans="3:15">
+    <row r="37" spans="3:15" ht="18">
       <c r="C37" s="47" t="s">
         <v>15</v>
       </c>
@@ -7746,7 +7750,7 @@
       <c r="J37" s="48"/>
       <c r="K37" s="49"/>
     </row>
-    <row r="38" spans="3:15">
+    <row r="38" spans="3:15" ht="18">
       <c r="C38" s="46">
         <v>550</v>
       </c>
@@ -7773,7 +7777,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="39" spans="3:15">
+    <row r="39" spans="3:15" ht="18">
       <c r="C39" s="45">
         <v>550</v>
       </c>
@@ -7799,10 +7803,10 @@
       <c r="K39" s="45">
         <v>2.1</v>
       </c>
-      <c r="N39" s="58"/>
-      <c r="O39" s="58"/>
-    </row>
-    <row r="40" spans="3:15">
+      <c r="N39" s="57"/>
+      <c r="O39" s="57"/>
+    </row>
+    <row r="40" spans="3:15" ht="18">
       <c r="C40" s="45">
         <v>550</v>
       </c>
@@ -7828,10 +7832,10 @@
       <c r="K40" s="45">
         <v>2</v>
       </c>
-      <c r="N40" s="58"/>
-      <c r="O40" s="58"/>
-    </row>
-    <row r="41" spans="3:15">
+      <c r="N40" s="57"/>
+      <c r="O40" s="57"/>
+    </row>
+    <row r="41" spans="3:15" ht="18">
       <c r="C41" s="45">
         <v>550</v>
       </c>
@@ -7857,10 +7861,10 @@
       <c r="K41" s="45">
         <v>1.8</v>
       </c>
-      <c r="N41" s="58"/>
-      <c r="O41" s="58"/>
-    </row>
-    <row r="42" spans="3:15">
+      <c r="N41" s="57"/>
+      <c r="O41" s="57"/>
+    </row>
+    <row r="42" spans="3:15" ht="18">
       <c r="C42" s="45">
         <v>550</v>
       </c>
@@ -7886,10 +7890,10 @@
       <c r="K42" s="45">
         <v>1.7</v>
       </c>
-      <c r="N42" s="58"/>
-      <c r="O42" s="58"/>
-    </row>
-    <row r="43" spans="3:15">
+      <c r="N42" s="57"/>
+      <c r="O42" s="57"/>
+    </row>
+    <row r="43" spans="3:15" ht="18">
       <c r="C43" s="45">
         <v>550</v>
       </c>
@@ -7915,10 +7919,10 @@
       <c r="K43" s="45">
         <v>1.6</v>
       </c>
-      <c r="N43" s="58"/>
-      <c r="O43" s="58"/>
-    </row>
-    <row r="44" spans="3:15">
+      <c r="N43" s="57"/>
+      <c r="O43" s="57"/>
+    </row>
+    <row r="44" spans="3:15" ht="18">
       <c r="C44" s="50">
         <v>550</v>
       </c>
@@ -7944,10 +7948,10 @@
       <c r="K44" s="50">
         <v>1.5</v>
       </c>
-      <c r="N44" s="58"/>
-      <c r="O44" s="58"/>
-    </row>
-    <row r="45" spans="3:15">
+      <c r="N44" s="57"/>
+      <c r="O44" s="57"/>
+    </row>
+    <row r="45" spans="3:15" ht="18">
       <c r="C45" s="54"/>
       <c r="D45" s="55"/>
       <c r="E45" s="55"/>
@@ -7957,10 +7961,10 @@
       <c r="I45" s="55"/>
       <c r="J45" s="55"/>
       <c r="K45" s="56"/>
-      <c r="N45" s="58"/>
-      <c r="O45" s="58"/>
-    </row>
-    <row r="46" spans="3:15">
+      <c r="N45" s="57"/>
+      <c r="O45" s="57"/>
+    </row>
+    <row r="46" spans="3:15" ht="18">
       <c r="C46" s="51"/>
       <c r="D46" s="52"/>
       <c r="E46" s="52"/>
@@ -7970,10 +7974,10 @@
       <c r="I46" s="52"/>
       <c r="J46" s="52"/>
       <c r="K46" s="53"/>
-      <c r="N46" s="58"/>
-      <c r="O46" s="58"/>
-    </row>
-    <row r="47" spans="3:15">
+      <c r="N46" s="57"/>
+      <c r="O46" s="57"/>
+    </row>
+    <row r="47" spans="3:15" ht="18">
       <c r="C47" s="51" t="s">
         <v>16</v>
       </c>
@@ -7985,10 +7989,10 @@
       <c r="I47" s="52"/>
       <c r="J47" s="52"/>
       <c r="K47" s="53"/>
-      <c r="N47" s="58"/>
-      <c r="O47" s="58"/>
-    </row>
-    <row r="48" spans="3:15">
+      <c r="N47" s="57"/>
+      <c r="O47" s="57"/>
+    </row>
+    <row r="48" spans="3:15" ht="18">
       <c r="C48" s="46">
         <v>1</v>
       </c>
@@ -8014,10 +8018,10 @@
         <v>300</v>
       </c>
       <c r="K48" s="46"/>
-      <c r="N48" s="58"/>
-      <c r="O48" s="58"/>
-    </row>
-    <row r="49" spans="3:15">
+      <c r="N48" s="57"/>
+      <c r="O48" s="57"/>
+    </row>
+    <row r="49" spans="3:15" ht="18">
       <c r="C49" s="45">
         <v>2</v>
       </c>
@@ -8043,10 +8047,10 @@
         <v>450</v>
       </c>
       <c r="K49" s="45"/>
-      <c r="N49" s="58"/>
+      <c r="N49" s="57"/>
       <c r="O49" s="57"/>
     </row>
-    <row r="50" spans="3:15">
+    <row r="50" spans="3:15" ht="18">
       <c r="C50" s="45">
         <v>3</v>
       </c>
@@ -8072,9 +8076,9 @@
         <v>600</v>
       </c>
       <c r="K50" s="45"/>
-      <c r="N50" s="58"/>
-    </row>
-    <row r="51" spans="3:15">
+      <c r="N50" s="57"/>
+    </row>
+    <row r="51" spans="3:15" ht="18">
       <c r="C51" s="50">
         <v>4</v>
       </c>
@@ -8100,9 +8104,9 @@
         <v>1000</v>
       </c>
       <c r="K51" s="50"/>
-      <c r="N51" s="58"/>
-    </row>
-    <row r="52" spans="3:15">
+      <c r="N51" s="57"/>
+    </row>
+    <row r="52" spans="3:15" ht="18">
       <c r="C52" s="54"/>
       <c r="D52" s="55"/>
       <c r="E52" s="55"/>
@@ -8112,9 +8116,9 @@
       <c r="I52" s="55"/>
       <c r="J52" s="55"/>
       <c r="K52" s="56"/>
-      <c r="N52" s="58"/>
-    </row>
-    <row r="53" spans="3:15">
+      <c r="N52" s="57"/>
+    </row>
+    <row r="53" spans="3:15" ht="18">
       <c r="C53" s="51"/>
       <c r="D53" s="52"/>
       <c r="E53" s="52"/>
@@ -8124,9 +8128,9 @@
       <c r="I53" s="52"/>
       <c r="J53" s="52"/>
       <c r="K53" s="53"/>
-      <c r="N53" s="58"/>
-    </row>
-    <row r="54" spans="3:15">
+      <c r="N53" s="57"/>
+    </row>
+    <row r="54" spans="3:15" ht="18">
       <c r="C54" s="51" t="s">
         <v>17</v>
       </c>
@@ -8138,9 +8142,9 @@
       <c r="I54" s="52"/>
       <c r="J54" s="52"/>
       <c r="K54" s="53"/>
-      <c r="N54" s="58"/>
-    </row>
-    <row r="55" spans="3:15">
+      <c r="N54" s="57"/>
+    </row>
+    <row r="55" spans="3:15" ht="18">
       <c r="C55" s="46">
         <v>1</v>
       </c>
@@ -8166,9 +8170,9 @@
         <v>300</v>
       </c>
       <c r="K55" s="46"/>
-      <c r="N55" s="58"/>
-    </row>
-    <row r="56" spans="3:15">
+      <c r="N55" s="57"/>
+    </row>
+    <row r="56" spans="3:15" ht="18">
       <c r="C56" s="45">
         <v>2</v>
       </c>
@@ -8194,9 +8198,9 @@
         <v>400</v>
       </c>
       <c r="K56" s="45"/>
-      <c r="N56" s="58"/>
-    </row>
-    <row r="57" spans="3:15">
+      <c r="N56" s="57"/>
+    </row>
+    <row r="57" spans="3:15" ht="18">
       <c r="C57" s="45">
         <v>3</v>
       </c>
@@ -8223,7 +8227,7 @@
       </c>
       <c r="K57" s="45"/>
     </row>
-    <row r="58" spans="3:15">
+    <row r="58" spans="3:15" ht="18">
       <c r="C58" s="50">
         <v>4</v>
       </c>
@@ -8250,7 +8254,7 @@
       </c>
       <c r="K58" s="50"/>
     </row>
-    <row r="59" spans="3:15">
+    <row r="59" spans="3:15" ht="18">
       <c r="C59" s="54"/>
       <c r="D59" s="55"/>
       <c r="E59" s="55"/>
@@ -8261,7 +8265,7 @@
       <c r="J59" s="55"/>
       <c r="K59" s="56"/>
     </row>
-    <row r="60" spans="3:15">
+    <row r="60" spans="3:15" ht="18">
       <c r="C60" s="51"/>
       <c r="D60" s="52"/>
       <c r="E60" s="52"/>
@@ -8272,7 +8276,7 @@
       <c r="J60" s="52"/>
       <c r="K60" s="53"/>
     </row>
-    <row r="61" spans="3:15">
+    <row r="61" spans="3:15" ht="18">
       <c r="C61" s="51" t="s">
         <v>24</v>
       </c>
@@ -8285,7 +8289,7 @@
       <c r="J61" s="52"/>
       <c r="K61" s="53"/>
     </row>
-    <row r="62" spans="3:15">
+    <row r="62" spans="3:15" ht="18">
       <c r="C62" s="46">
         <v>1</v>
       </c>
@@ -8312,7 +8316,7 @@
       </c>
       <c r="K62" s="46"/>
     </row>
-    <row r="63" spans="3:15">
+    <row r="63" spans="3:15" ht="18">
       <c r="C63" s="45">
         <v>2</v>
       </c>
@@ -8339,7 +8343,7 @@
       </c>
       <c r="K63" s="45"/>
     </row>
-    <row r="64" spans="3:15">
+    <row r="64" spans="3:15" ht="18">
       <c r="C64" s="45">
         <v>3</v>
       </c>
@@ -8366,7 +8370,7 @@
       </c>
       <c r="K64" s="45"/>
     </row>
-    <row r="65" spans="3:11">
+    <row r="65" spans="3:11" ht="18">
       <c r="C65" s="45">
         <v>4</v>
       </c>
@@ -8432,9 +8436,9 @@
       <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="13" max="13" width="39.296875" style="28" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="39.33203125" style="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22">
@@ -9044,7 +9048,7 @@
     <row r="13" spans="1:22">
       <c r="G13" s="9"/>
     </row>
-    <row r="14" spans="1:22" ht="16.2" thickBot="1">
+    <row r="14" spans="1:22" ht="17" thickBot="1">
       <c r="G14" s="9"/>
     </row>
     <row r="15" spans="1:22" s="14" customFormat="1">
@@ -9514,13 +9518,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93F1BF91-8CAF-244E-B6BF-FE8B646402AF}">
   <dimension ref="A1:AB49"/>
   <sheetViews>
-    <sheetView zoomScale="64" workbookViewId="0">
+    <sheetView zoomScale="83" workbookViewId="0">
       <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="13" max="13" width="10.796875" style="28"/>
+    <col min="13" max="13" width="10.83203125" style="28"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28">
@@ -10267,7 +10271,7 @@
       <c r="AA13" s="23"/>
       <c r="AB13" s="23"/>
     </row>
-    <row r="14" spans="1:28" ht="16.2" thickBot="1">
+    <row r="14" spans="1:28" ht="17" thickBot="1">
       <c r="A14" s="23"/>
       <c r="B14" s="23"/>
       <c r="C14" s="23"/>
@@ -10415,7 +10419,7 @@
       <c r="AA17" s="23"/>
       <c r="AB17" s="23"/>
     </row>
-    <row r="18" spans="1:28" ht="16.2" thickBot="1">
+    <row r="18" spans="1:28" ht="17" thickBot="1">
       <c r="A18" s="23"/>
       <c r="B18" s="23"/>
       <c r="C18" s="23"/>
@@ -11659,18 +11663,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4473C636-8F8B-734A-9EFB-C73EEF4CFCCF}">
   <dimension ref="A1:AB30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="56" workbookViewId="0">
-      <selection activeCell="O20" sqref="O20"/>
+    <sheetView tabSelected="1" topLeftCell="M5" zoomScale="144" workbookViewId="0">
+      <selection activeCell="S13" sqref="S13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="2" max="2" width="47" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.69921875" customWidth="1"/>
-    <col min="13" max="13" width="39.296875" style="28" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" customWidth="1"/>
+    <col min="13" max="13" width="39.33203125" style="28" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="2.796875" customWidth="1"/>
-    <col min="24" max="24" width="10.796875" style="28"/>
+    <col min="23" max="23" width="2.83203125" customWidth="1"/>
+    <col min="24" max="24" width="10.83203125" style="28"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24">
@@ -12339,7 +12343,7 @@
       <c r="U13" s="23"/>
       <c r="V13" s="23"/>
     </row>
-    <row r="14" spans="1:24" ht="16.2" thickBot="1">
+    <row r="14" spans="1:24" ht="17" thickBot="1">
       <c r="A14" s="23"/>
       <c r="B14" s="23"/>
       <c r="C14" s="23"/>
@@ -12363,7 +12367,7 @@
       <c r="U14" s="23"/>
       <c r="V14" s="23"/>
     </row>
-    <row r="15" spans="1:24" s="19" customFormat="1" ht="16.2" thickBot="1">
+    <row r="15" spans="1:24" s="19" customFormat="1" ht="17" thickBot="1">
       <c r="A15" s="35"/>
       <c r="B15" s="35" t="s">
         <v>26</v>
@@ -13085,7 +13089,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="2:28" ht="16.2" thickBot="1"/>
+    <row r="28" spans="2:28" ht="17" thickBot="1"/>
     <row r="29" spans="2:28" s="14" customFormat="1">
       <c r="M29" s="29" t="s">
         <v>33</v>

</xml_diff>